<commit_message>
Matouqin: update test data
</commit_message>
<xml_diff>
--- a/models/matouqin/Data/dat1.xlsx
+++ b/models/matouqin/Data/dat1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\model\yayue\models\matouqin\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE81A309-35D8-4ED8-8531-2B775539BD9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE1F1F3-717A-4F02-958B-AE302D377603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" activeTab="4" xr2:uid="{AEEBE647-0CC9-4089-B5C6-ED9E548DECB5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" activeTab="5" xr2:uid="{AEEBE647-0CC9-4089-B5C6-ED9E548DECB5}"/>
   </bookViews>
   <sheets>
     <sheet name="cf" sheetId="1" r:id="rId1"/>
@@ -1307,11 +1307,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>hmi</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>Tank2</t>
   </si>
   <si>
-    <t>Tank2</t>
+    <t>hini</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -71915,7 +71915,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -71986,8 +71986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D39AA25D-8DDD-4DE2-BB31-FBA4668F09F8}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView topLeftCell="B1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -72029,7 +72029,7 @@
         <v>4.5</v>
       </c>
       <c r="E2" s="1">
-        <v>7</v>
+        <v>0.7</v>
       </c>
       <c r="F2" s="1">
         <v>0.05</v>
@@ -72046,8 +72046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{577A8CDB-DCE2-4409-ABF8-20369696E92F}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -72066,7 +72066,7 @@
         <v>8</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>3</v>
@@ -72118,7 +72118,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3">
         <v>500</v>
@@ -72160,7 +72160,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>

</xml_diff>